<commit_message>
automate basic process with create order
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/TimeCompression.xlsx
+++ b/src/main/resources/excel/TimeCompression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POLIGON\process-executor\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934AD94C-75F2-4D1D-A1F6-7396A5D2E459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3066A43F-2CF4-412C-9E55-5E6112CE4421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15590" yWindow="2750" windowWidth="24230" windowHeight="18370" xr2:uid="{450F3A6C-B4B9-401E-BE9B-ADF9BB967B33}"/>
+    <workbookView xWindow="12060" yWindow="2740" windowWidth="24230" windowHeight="18370" xr2:uid="{450F3A6C-B4B9-401E-BE9B-ADF9BB967B33}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Поставка материалов</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Операций на кон. Изделие</t>
+  </si>
+  <si>
+    <t>Между запусками в 1 заказе</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -151,6 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -465,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F4F369-3CA8-4298-BB05-1AECDF55D2FF}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -520,7 +524,7 @@
         <v>10800</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E14" si="0">$D3/$B$18</f>
+        <f t="shared" ref="E3:E15" si="0">$D3/$B$18</f>
         <v>216</v>
       </c>
     </row>
@@ -728,6 +732,9 @@
         <v>60</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E15" s="2"/>
+    </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
@@ -736,13 +743,40 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <f>E17*B18</f>
+        <v>500</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
         <f>MIN(D2:D14)</f>
         <v>50</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18">
+        <f>SUM(E2:E15)</f>
+        <v>543</v>
+      </c>
+      <c r="F18">
+        <f>SUM(E4:E14)</f>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F19">
+        <f>SUM(E5:E14)</f>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
accelerate process runner from 10 s to 6 s and accelerate purchasers
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/TimeCompression.xlsx
+++ b/src/main/resources/excel/TimeCompression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POLIGON\process-executor\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3066A43F-2CF4-412C-9E55-5E6112CE4421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1066073E-A019-467C-9827-A3690024FB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12060" yWindow="2740" windowWidth="24230" windowHeight="18370" xr2:uid="{450F3A6C-B4B9-401E-BE9B-ADF9BB967B33}"/>
+    <workbookView xWindow="12510" yWindow="4670" windowWidth="24230" windowHeight="18370" xr2:uid="{450F3A6C-B4B9-401E-BE9B-ADF9BB967B33}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,11 +507,11 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2">
-        <v>7200</v>
+        <v>900</v>
       </c>
       <c r="E2" s="2">
         <f>$D2/$B$18</f>
-        <v>144</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -521,11 +521,11 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3">
-        <v>10800</v>
+        <v>1800</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E15" si="0">$D3/$B$18</f>
-        <v>216</v>
+        <f t="shared" ref="E3:E14" si="0">$D3/$B$18</f>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -535,11 +535,11 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4">
-        <v>3600</v>
+        <v>900</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -749,10 +749,10 @@
       </c>
       <c r="D17">
         <f>E17*B18</f>
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -766,11 +766,11 @@
       <c r="D18" s="6"/>
       <c r="E18">
         <f>SUM(E2:E15)</f>
-        <v>543</v>
+        <v>183</v>
       </c>
       <c r="F18">
         <f>SUM(E4:E14)</f>
-        <v>183</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>